<commit_message>
Further development on algorithm. Parallel.For ArgumentOutofRangeException thrown on execution
</commit_message>
<xml_diff>
--- a/Flowchart_Routing.xlsx
+++ b/Flowchart_Routing.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8910" xr2:uid="{6EDB68E0-EBBD-44C9-A24D-FB29B23BDC17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8910" activeTab="1" xr2:uid="{6EDB68E0-EBBD-44C9-A24D-FB29B23BDC17}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Target Algorithm" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,18 +25,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Old Concept, detailed. Approx. 0.9.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -62,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -722,7 +734,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1876425" y="2000250"/>
+          <a:off x="1876425" y="2143125"/>
           <a:ext cx="1369358" cy="836060"/>
           <a:chOff x="2943225" y="1971675"/>
           <a:chExt cx="1369358" cy="836060"/>
@@ -1437,7 +1449,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7562850" y="4095749"/>
+          <a:off x="7562850" y="4238624"/>
           <a:ext cx="1828800" cy="904875"/>
           <a:chOff x="7562850" y="4095749"/>
           <a:chExt cx="1828800" cy="904875"/>
@@ -1875,7 +1887,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4963645" y="7458075"/>
+          <a:off x="4963645" y="7600950"/>
           <a:ext cx="2826684" cy="1847850"/>
           <a:chOff x="5314949" y="7458075"/>
           <a:chExt cx="2826684" cy="1847850"/>
@@ -2980,7 +2992,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5135563" y="11386344"/>
+          <a:off x="5135563" y="11529219"/>
           <a:ext cx="1259681" cy="809867"/>
           <a:chOff x="8167688" y="11203781"/>
           <a:chExt cx="1259681" cy="809867"/>
@@ -3814,7 +3826,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10981531" y="9576594"/>
+          <a:off x="10981531" y="9719469"/>
           <a:ext cx="4198938" cy="2274094"/>
           <a:chOff x="10791031" y="9655969"/>
           <a:chExt cx="4198938" cy="2274094"/>
@@ -4286,6 +4298,705 @@
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val -2241"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Flussdiagramm: Prozess 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{122A2A73-CE22-4715-98D4-38732BBB98D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4460081" y="1828800"/>
+          <a:ext cx="2095500" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Calculate Route from Start to End</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Flussdiagramm: Prozess 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E373F7-1BA7-4C50-B769-9E364F4B1CF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4460081" y="2447925"/>
+          <a:ext cx="2095500" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Add fix Include Geocaches</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Flussdiagramm: Prozess 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71C20C89-701E-443B-89EE-4DF23791DD34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4460081" y="3076575"/>
+          <a:ext cx="2095500" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Resolve top x geocaches</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Flussdiagramm: Prozess 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4B439E-CBE0-4FB7-BFC9-A88B77B7A0B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4460081" y="3695700"/>
+          <a:ext cx="2095500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Calculate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> n variants of the route until each reaches a route length of 60-80% of the total length. Choose route that has most points in reach.</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Flussdiagramm: Prozess 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8667C242-C85F-4F48-B919-85510F032866}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4460081" y="4843463"/>
+          <a:ext cx="2095500" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Resolve all</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> not added geocaches in reach</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Flussdiagramm: Prozess 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B4256F0-3528-4B01-B80B-90B58C3AF726}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4460081" y="5676900"/>
+          <a:ext cx="2095500" cy="1314450"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Calculate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> final route by choosing the top rated geocache, whose distance to the route is less than the remainng distance divided by  x, plus a tolerance variable y. If it increases the route's  total points keep it, else forget it.</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>53182</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>44449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>65882</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>34924</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Verbinder: gewinkelt 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58B7049E-29F3-47B8-A324-58928CE9BBB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5322094" y="2890837"/>
+          <a:ext cx="371475" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>53181</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>173038</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>65881</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Verbinder: gewinkelt 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A9D4334-D5CA-4B48-91F5-F7863D3834D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="2"/>
+          <a:endCxn id="9" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5324475" y="5493544"/>
+          <a:ext cx="366712" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>53181</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>65881</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Verbinder: gewinkelt 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EE8C4CC-8121-4F3D-9E3B-E3CA61E4E485}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="7" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5326856" y="3514725"/>
+          <a:ext cx="361950" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>53182</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>65882</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>87312</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Verbinder: gewinkelt 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4577EB97-AC88-4CB3-A6CF-049C70A3AE12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="2"/>
+          <a:endCxn id="8" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5410200" y="4745831"/>
+          <a:ext cx="195263" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>53181</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>187325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>65881</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Verbinder: gewinkelt 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{369A69DE-1706-4AB1-9E78-F17DC58ECEDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5326856" y="2266950"/>
+          <a:ext cx="361950" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="19050">
@@ -4639,14 +5350,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C373B2-02FC-4AE8-9CD0-C75B74C333F5}">
-  <dimension ref="C75"/>
+  <dimension ref="C3:E75"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="BK67" sqref="BK67"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="3" spans="5:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>0</v>
@@ -4654,6 +5370,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC082A9-810F-4094-A15B-2684AFE42598}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="AU15" sqref="AU15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>